<commit_message>
excel file and scraping
</commit_message>
<xml_diff>
--- a/MentorMindWork.xlsx
+++ b/MentorMindWork.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -259,6 +259,24 @@
   </si>
   <si>
     <t>Modified in Recommendation challenges</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>vistaar</t>
+  </si>
+  <si>
+    <t>13/3/2019</t>
+  </si>
+  <si>
+    <t>owncloud</t>
+  </si>
+  <si>
+    <t>14/4/2019</t>
+  </si>
+  <si>
+    <t>narratives</t>
   </si>
 </sst>
 </file>
@@ -336,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -377,6 +395,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
@@ -1245,12 +1264,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="14">
+        <v>43802</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>